<commit_message>
cleanup templates and save increases in snowflake tables
</commit_message>
<xml_diff>
--- a/excel_templates/eps.xlsx
+++ b/excel_templates/eps.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2357059C-41D6-4BA4-9436-CCFCDF3ED41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC7A49-0B55-4F82-98FD-44D4E0AAD434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,12 +15,12 @@
     <sheet name="ePacket Zone List" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ePacket Zone List'!$A$2:$C$28</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ePacket!$B$1:$E$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ePacket Zone List'!$A$2:$C$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ePacket!$B$1:$E$25</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'ePacket DDP'!$B$1:$E$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'ePacket Oz to Lb Chart'!$B$1:$N$43</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'ePacket Rate Calculator'!$B$1:$G$38</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'ePacket Zone List'!$A$1:$C$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'ePacket Rate Calculator'!$B$1:$G$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'ePacket Zone List'!$A$1:$C$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
   <si>
     <t>Destination</t>
   </si>
@@ -325,13 +325,49 @@
     <t>asdf - 2022</t>
   </si>
   <si>
-    <t>Effective 1/23/2023</t>
-  </si>
-  <si>
     <t>ePacket Zone List - 2023</t>
   </si>
   <si>
     <t>2023 Rate Calculator</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Effective 1/22/2023</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Thailand</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1216,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B7:E27"/>
+  <dimension ref="B7:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1297,43 +1333,48 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="B22" s="2"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="23" t="s">
+    <row r="24" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
+    </row>
+    <row r="28" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="B7:E7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
@@ -1410,7 +1451,7 @@
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1454,7 +1495,7 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O38"/>
+  <dimension ref="B1:O45"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:G6"/>
@@ -1491,7 +1532,7 @@
     </row>
     <row r="6" spans="2:15" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -1563,58 +1604,59 @@
         <v>1</v>
       </c>
       <c r="E11" s="17" t="e">
-        <f>VLOOKUP($B11,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B11,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F11" s="17" t="e">
-        <f>VLOOKUP($B11,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B11,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G11" s="17" t="e">
-        <f t="shared" ref="G11:G36" si="0">IF(OR(AND($F$7="Oz",$G$7&lt;=70.4),AND($F$7="Lb",$G$7&lt;=4.4),AND($F$7="Kg",$G$7&lt;=2)),ROUND($E11+IFERROR($F11*CONVERT($G$7,CONCATENATE(LOWER($F$7),"m"),"lbm"),$F11*CONVERT($G$7,CONCATENATE(LOWER($F$7)),"lbm")),2),"Exceeds Max Weight")</f>
+        <f t="shared" ref="G11:G42" si="0">IF(OR(AND($F$7="Oz",$G$7&lt;=70.4),AND($F$7="Lb",$G$7&lt;=4.4),AND($F$7="Kg",$G$7&lt;=2)),ROUND($E11+IFERROR($F11*CONVERT($G$7,CONCATENATE(LOWER($F$7),"m"),"lbm"),$F11*CONVERT($G$7,CONCATENATE(LOWER($F$7)),"lbm")),2),"Exceeds Max Weight")</f>
         <v>#N/A</v>
       </c>
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="E12" s="18" t="e">
-        <f>VLOOKUP($B12,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B12,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F12" s="18" t="e">
-        <f>VLOOKUP($B12,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B12,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G12" s="18" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="17" t="e">
-        <f>VLOOKUP($B13,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B13,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F13" s="17" t="e">
-        <f>VLOOKUP($B13,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B13,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G13" s="17" t="e">
@@ -1627,64 +1669,64 @@
         <v>7</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E14" s="18" t="e">
-        <f>VLOOKUP($B14,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B14,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F14" s="18" t="e">
-        <f>VLOOKUP($B14,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B14,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G14" s="18" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E15" s="17" t="e">
-        <f>VLOOKUP($B15,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B15,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F15" s="17" t="e">
-        <f>VLOOKUP($B15,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B15,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G15" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E16" s="18" t="e">
-        <f>VLOOKUP($B16,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B16,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F16" s="18" t="e">
-        <f>VLOOKUP($B16,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B16,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G16" s="18" t="e">
@@ -1694,20 +1736,20 @@
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="E17" s="17" t="e">
-        <f>VLOOKUP($B17,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B17,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F17" s="17" t="e">
-        <f>VLOOKUP($B17,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B17,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G17" s="17" t="e">
@@ -1720,17 +1762,17 @@
         <v>8</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E18" s="18" t="e">
-        <f>VLOOKUP($B18,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B18,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F18" s="18" t="e">
-        <f>VLOOKUP($B18,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B18,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G18" s="18" t="e">
@@ -1743,17 +1785,17 @@
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E19" s="17" t="e">
-        <f>VLOOKUP($B19,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B19,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F19" s="17" t="e">
-        <f>VLOOKUP($B19,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B19,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G19" s="17" t="e">
@@ -1763,20 +1805,20 @@
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E20" s="18" t="e">
-        <f>VLOOKUP($B20,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B20,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F20" s="18" t="e">
-        <f>VLOOKUP($B20,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B20,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G20" s="18" t="e">
@@ -1786,20 +1828,20 @@
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E21" s="17" t="e">
-        <f>VLOOKUP($B21,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B21,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F21" s="17" t="e">
-        <f>VLOOKUP($B21,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B21,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G21" s="17" t="e">
@@ -1809,20 +1851,20 @@
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E22" s="18" t="e">
-        <f>VLOOKUP($B22,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B22,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F22" s="18" t="e">
-        <f>VLOOKUP($B22,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B22,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G22" s="18" t="e">
@@ -1835,17 +1877,17 @@
         <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E23" s="17" t="e">
-        <f>VLOOKUP($B23,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B23,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F23" s="17" t="e">
-        <f>VLOOKUP($B23,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B23,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G23" s="17" t="e">
@@ -1858,17 +1900,17 @@
         <v>9</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E24" s="18" t="e">
-        <f>VLOOKUP($B24,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B24,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F24" s="18" t="e">
-        <f>VLOOKUP($B24,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B24,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G24" s="18" t="e">
@@ -1881,17 +1923,17 @@
         <v>9</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E25" s="17" t="e">
-        <f>VLOOKUP($B25,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B25,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F25" s="17" t="e">
-        <f>VLOOKUP($B25,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B25,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G25" s="17" t="e">
@@ -1904,17 +1946,17 @@
         <v>9</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="E26" s="18" t="e">
-        <f>VLOOKUP($B26,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B26,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F26" s="18" t="e">
-        <f>VLOOKUP($B26,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B26,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G26" s="18" t="e">
@@ -1924,20 +1966,20 @@
     </row>
     <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E27" s="17" t="e">
-        <f>VLOOKUP($B27,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B27,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F27" s="17" t="e">
-        <f>VLOOKUP($B27,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B27,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G27" s="17" t="e">
@@ -1947,20 +1989,20 @@
     </row>
     <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="E28" s="18" t="e">
-        <f>VLOOKUP($B28,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B28,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F28" s="18" t="e">
-        <f>VLOOKUP($B28,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B28,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G28" s="18" t="e">
@@ -1970,20 +2012,20 @@
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E29" s="17" t="e">
-        <f>VLOOKUP($B29,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B29,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F29" s="17" t="e">
-        <f>VLOOKUP($B29,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B29,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G29" s="17" t="e">
@@ -1993,20 +2035,20 @@
     </row>
     <row r="30" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E30" s="18" t="e">
-        <f>VLOOKUP($B30,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B30,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F30" s="18" t="e">
-        <f>VLOOKUP($B30,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B30,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G30" s="18" t="e">
@@ -2016,20 +2058,20 @@
     </row>
     <row r="31" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="E31" s="17" t="e">
-        <f>VLOOKUP($B31,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B31,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F31" s="17" t="e">
-        <f>VLOOKUP($B31,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B31,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G31" s="17" t="e">
@@ -2039,20 +2081,20 @@
     </row>
     <row r="32" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E32" s="18" t="e">
-        <f>VLOOKUP($B32,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B32,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F32" s="18" t="e">
-        <f>VLOOKUP($B32,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B32,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G32" s="18" t="e">
@@ -2062,20 +2104,20 @@
     </row>
     <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E33" s="17" t="e">
-        <f>VLOOKUP($B33,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B33,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F33" s="17" t="e">
-        <f>VLOOKUP($B33,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B33,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G33" s="17" t="e">
@@ -2085,20 +2127,20 @@
     </row>
     <row r="34" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="E34" s="18" t="e">
-        <f>VLOOKUP($B34,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B34,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F34" s="18" t="e">
-        <f>VLOOKUP($B34,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B34,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G34" s="18" t="e">
@@ -2108,20 +2150,20 @@
     </row>
     <row r="35" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E35" s="17" t="e">
-        <f>VLOOKUP($B35,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B35,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F35" s="17" t="e">
-        <f>VLOOKUP($B35,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B35,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G35" s="17" t="e">
@@ -2131,20 +2173,20 @@
     </row>
     <row r="36" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="14">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E36" s="18" t="e">
-        <f>VLOOKUP($B36,ePacket!$B$11:$E$21,3,FALSE)</f>
+        <f>VLOOKUP($B36,ePacket!$B$11:$E$23,3,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F36" s="18" t="e">
-        <f>VLOOKUP($B36,ePacket!$B$11:$E$21,4,FALSE)</f>
+        <f>VLOOKUP($B36,ePacket!$B$11:$E$23,4,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="G36" s="18" t="e">
@@ -2153,26 +2195,172 @@
       </c>
     </row>
     <row r="37" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-    </row>
-    <row r="38" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="26" t="s">
+      <c r="B37" s="3">
+        <v>15</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="17" t="e">
+        <f>VLOOKUP($B37,ePacket!$B$11:$E$23,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F37" s="17" t="e">
+        <f>VLOOKUP($B37,ePacket!$B$11:$E$23,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G37" s="17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="14">
+        <v>16</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="18" t="e">
+        <f>VLOOKUP($B38,ePacket!$B$11:$E$23,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F38" s="18" t="e">
+        <f>VLOOKUP($B38,ePacket!$B$11:$E$23,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G38" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>17</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="17" t="e">
+        <f>VLOOKUP($B39,ePacket!$B$11:$E$23,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F39" s="17" t="e">
+        <f>VLOOKUP($B39,ePacket!$B$11:$E$23,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G39" s="17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="14">
+        <v>18</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="18" t="e">
+        <f>VLOOKUP($B40,ePacket!$B$11:$E$23,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F40" s="18" t="e">
+        <f>VLOOKUP($B40,ePacket!$B$11:$E$23,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G40" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>18</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="17" t="e">
+        <f>VLOOKUP($B41,ePacket!$B$11:$E$23,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F41" s="17" t="e">
+        <f>VLOOKUP($B41,ePacket!$B$11:$E$23,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G41" s="17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="14">
+        <v>20</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="18" t="e">
+        <f>VLOOKUP($B42,ePacket!$B$11:$E$23,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F42" s="18" t="e">
+        <f>VLOOKUP($B42,ePacket!$B$11:$E$23,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G42" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+    </row>
+    <row r="44" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+    </row>
+    <row r="45" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tWOsHC9r8EAcc1Fa7NrzwIRPNzR3Y/4+Mh6tivsXcawM9yTXDvKH3eHFmR1wHCLWoeqTmS9ZEpGY3IrAZ6nClg==" saltValue="JElV3aPe8nCQV1eK+a9+Fg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Mdht4DtTATqYoYzQmPYP9laxWDOQtRGUpJlJFbUC59yLH01gctpMqsrAjv2GIoK3GCYvpPiHZlCuTO5EigsBLg==" saltValue="Wg/EZUsirQBbqEWbeX4Oeg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="5">
     <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B7:E7"/>
   </mergeCells>
@@ -2197,7 +2385,7 @@
   </sheetPr>
   <dimension ref="B7:Q43"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:N7"/>
     </sheetView>
   </sheetViews>
@@ -2823,7 +3011,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2841,7 +3029,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -2871,22 +3059,22 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="C4" s="14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3">
         <v>7</v>
@@ -2895,10 +3083,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C6" s="14">
         <v>7</v>
@@ -2907,10 +3095,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3">
         <v>7</v>
@@ -2919,34 +3107,34 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C8" s="14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" s="14">
         <v>8</v>
@@ -2955,10 +3143,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3">
         <v>8</v>
@@ -2967,46 +3155,46 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C12" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C13" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C14" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3">
         <v>9</v>
@@ -3015,10 +3203,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C16" s="14">
         <v>9</v>
@@ -3027,10 +3215,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>9</v>
@@ -3039,10 +3227,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="C18" s="14">
         <v>9</v>
@@ -3051,135 +3239,196 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C19" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="C20" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C21" s="3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C22" s="14">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="C23" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C24" s="14">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C25" s="3">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="C26" s="14">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C27" s="3">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="14">
+        <v>12</v>
+      </c>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3">
+        <v>15</v>
+      </c>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B34" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C34" s="14">
         <v>20</v>
       </c>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
     </row>
   </sheetData>
   <sheetProtection autoFilter="0"/>
-  <autoFilter ref="A2:C28" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <mergeCells count="2">
+  <autoFilter ref="A2:C29" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A29:C29"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
epacket ddp now on same sheet as epacket
</commit_message>
<xml_diff>
--- a/excel_templates/eps.xlsx
+++ b/excel_templates/eps.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC7A49-0B55-4F82-98FD-44D4E0AAD434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4B3899-2B88-4622-B5FB-16902DAF5E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ePacket" sheetId="8" r:id="rId1"/>
@@ -673,13 +673,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="CountryEven" xfId="6" xr:uid="{8DB1E861-031D-4765-A63D-3452F542C9C2}"/>
-    <cellStyle name="CountryOdd" xfId="5" xr:uid="{3310C328-04FE-4C18-A6BF-7AFF610A570C}"/>
+    <cellStyle name="CountryEven" xfId="5" xr:uid="{3310C328-04FE-4C18-A6BF-7AFF610A570C}"/>
+    <cellStyle name="CountryOdd" xfId="6" xr:uid="{8DB1E861-031D-4765-A63D-3452F542C9C2}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="RateEven" xfId="2" xr:uid="{F4873094-777D-4F14-B29C-C73E7192224B}"/>
-    <cellStyle name="RateOdd" xfId="1" xr:uid="{06184AEF-5B8B-4CEF-9B5B-2F82DFE38F8B}"/>
-    <cellStyle name="ZoneEven" xfId="4" xr:uid="{B52D5065-82E8-4A96-B9C4-F95280A99CCD}"/>
-    <cellStyle name="ZoneOdd" xfId="3" xr:uid="{6FE8A28A-AA60-4F45-9070-36F3EEEE2722}"/>
+    <cellStyle name="RateEven" xfId="1" xr:uid="{06184AEF-5B8B-4CEF-9B5B-2F82DFE38F8B}"/>
+    <cellStyle name="RateOdd" xfId="2" xr:uid="{F4873094-777D-4F14-B29C-C73E7192224B}"/>
+    <cellStyle name="ZoneEven" xfId="3" xr:uid="{6FE8A28A-AA60-4F45-9070-36F3EEEE2722}"/>
+    <cellStyle name="ZoneOdd" xfId="4" xr:uid="{B52D5065-82E8-4A96-B9C4-F95280A99CCD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1219,7 +1219,7 @@
   <dimension ref="B7:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>